<commit_message>
Se Agregan adicionales de tablas
</commit_message>
<xml_diff>
--- a/SILESWEB/DOCUMENTACION/Estructura de las tablas.xlsx
+++ b/SILESWEB/DOCUMENTACION/Estructura de las tablas.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredy Sarmiento\Documents\SILESWEB\DocumentacionSiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SILESWEB\SILESWEB\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F624A61-0F25-4175-9F31-9A143EA76101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9192" uniqueCount="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9373" uniqueCount="1073">
   <si>
     <t>nIdPEROP</t>
   </si>
@@ -3233,11 +3234,47 @@
   <si>
     <t>T_PRD_DET_FOM2_DetalleComponentesFormulasMaestras</t>
   </si>
+  <si>
+    <t>T_PRD_DET_FOM3_DetalleCostosIndirectosFabricacionFormulasMaestras</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_FOM5_DetalleAnalisis</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_LIM1_DetalleListadoFormulaMaestra</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_LIM2_DetalleListadoMateriales</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_LIM3_DetalleListadoMaterialesOperaciones</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_LIM4_DetalleListadoMaterialesCIF</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_ODP1_DetalleOrdenProduccion</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_ODP2_DetalleOrdenOperacion</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_ODP3_DetalleCIF</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_ODP4_ResumenOP</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_ODP5_DetalleAnalisis</t>
+  </si>
+  <si>
+    <t>T_PRD_DET_RCI1_DetalleRegistroCIF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3353,7 +3390,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Hoja1" xfId="1"/>
+    <cellStyle name="Normal_Hoja1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -3373,16 +3410,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:F1915" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:F1915" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="TABLA"/>
-    <tableColumn id="4" name="Nombre_tabla" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TABLA"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Nombre_tabla" dataDxfId="0">
       <calculatedColumnFormula>VLOOKUP(Tabla2[[#This Row],[TABLA]],Hoja1!$B$2:$C$131,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="NOMBRE_CAMPO"/>
-    <tableColumn id="3" name="TIPO DE DATOS"/>
-    <tableColumn id="5" name="TIPO DE DATOS SQL"/>
-    <tableColumn id="6" name="Nueva Tabla"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE_CAMPO"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TIPO DE DATOS"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TIPO DE DATOS SQL"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nueva Tabla"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3650,7 +3687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5503,11 +5540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1915"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1241" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1264" sqref="F1264"/>
+    <sheetView tabSelected="1" topLeftCell="A1598" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1494" sqref="F1494"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31695,8 +31732,11 @@
       <c r="E1264" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1264" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1265" t="s">
         <v>379</v>
       </c>
@@ -31713,8 +31753,11 @@
       <c r="E1265" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1265" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1266" t="s">
         <v>379</v>
       </c>
@@ -31731,8 +31774,11 @@
       <c r="E1266" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1266" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1267" t="s">
         <v>379</v>
       </c>
@@ -31749,8 +31795,11 @@
       <c r="E1267" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1267" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1268" t="s">
         <v>379</v>
       </c>
@@ -31767,8 +31816,11 @@
       <c r="E1268" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1268" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1269" t="s">
         <v>379</v>
       </c>
@@ -31785,8 +31837,11 @@
       <c r="E1269" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1269" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1270" t="s">
         <v>379</v>
       </c>
@@ -31803,8 +31858,11 @@
       <c r="E1270" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1270" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1271" t="s">
         <v>382</v>
       </c>
@@ -31821,8 +31879,11 @@
       <c r="E1271" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1271" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1272" t="s">
         <v>382</v>
       </c>
@@ -31839,8 +31900,11 @@
       <c r="E1272" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1272" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1273" t="s">
         <v>382</v>
       </c>
@@ -31857,8 +31921,11 @@
       <c r="E1273" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1273" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1274" t="s">
         <v>382</v>
       </c>
@@ -31875,8 +31942,11 @@
       <c r="E1274" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1274" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1275" t="s">
         <v>382</v>
       </c>
@@ -31893,8 +31963,11 @@
       <c r="E1275" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1275" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1276" t="s">
         <v>382</v>
       </c>
@@ -31911,8 +31984,11 @@
       <c r="E1276" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1276" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1277" t="s">
         <v>405</v>
       </c>
@@ -31929,8 +32005,11 @@
       <c r="E1277" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1277" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1278" t="s">
         <v>405</v>
       </c>
@@ -31947,8 +32026,11 @@
       <c r="E1278" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1278" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1279" t="s">
         <v>405</v>
       </c>
@@ -31965,8 +32047,11 @@
       <c r="E1279" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1279" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1280" t="s">
         <v>405</v>
       </c>
@@ -31983,8 +32068,11 @@
       <c r="E1280" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1280" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1281" t="s">
         <v>405</v>
       </c>
@@ -32001,8 +32089,11 @@
       <c r="E1281" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1281" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1282" t="s">
         <v>405</v>
       </c>
@@ -32019,8 +32110,11 @@
       <c r="E1282" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1282" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1283" t="s">
         <v>405</v>
       </c>
@@ -32037,8 +32131,11 @@
       <c r="E1283" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1283" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1284" t="s">
         <v>405</v>
       </c>
@@ -32055,8 +32152,11 @@
       <c r="E1284" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1284" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1285" t="s">
         <v>405</v>
       </c>
@@ -32073,8 +32173,11 @@
       <c r="E1285" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1285" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1286" t="s">
         <v>405</v>
       </c>
@@ -32091,8 +32194,11 @@
       <c r="E1286" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1286" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1287" t="s">
         <v>405</v>
       </c>
@@ -32109,8 +32215,11 @@
       <c r="E1287" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1287" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1288" t="s">
         <v>405</v>
       </c>
@@ -32127,8 +32236,11 @@
       <c r="E1288" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1288" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1289" t="s">
         <v>408</v>
       </c>
@@ -32145,8 +32257,11 @@
       <c r="E1289" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1289" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1290" t="s">
         <v>408</v>
       </c>
@@ -32163,8 +32278,11 @@
       <c r="E1290" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1290" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1291" t="s">
         <v>408</v>
       </c>
@@ -32181,8 +32299,11 @@
       <c r="E1291" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1291" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1292" t="s">
         <v>408</v>
       </c>
@@ -32199,8 +32320,11 @@
       <c r="E1292" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1292" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1293" t="s">
         <v>408</v>
       </c>
@@ -32217,8 +32341,11 @@
       <c r="E1293" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1293" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1294" t="s">
         <v>408</v>
       </c>
@@ -32235,8 +32362,11 @@
       <c r="E1294" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1294" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1295" t="s">
         <v>408</v>
       </c>
@@ -32253,8 +32383,11 @@
       <c r="E1295" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1295" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1296" t="s">
         <v>408</v>
       </c>
@@ -32271,8 +32404,11 @@
       <c r="E1296" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1296" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1297" t="s">
         <v>408</v>
       </c>
@@ -32289,8 +32425,11 @@
       <c r="E1297" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1297" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1298" t="s">
         <v>408</v>
       </c>
@@ -32307,8 +32446,11 @@
       <c r="E1298" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1298" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1299" t="s">
         <v>408</v>
       </c>
@@ -32325,8 +32467,11 @@
       <c r="E1299" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1299" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1300" t="s">
         <v>411</v>
       </c>
@@ -32343,8 +32488,11 @@
       <c r="E1300" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1300" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1301" t="s">
         <v>411</v>
       </c>
@@ -32361,8 +32509,11 @@
       <c r="E1301" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1301" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1302" t="s">
         <v>411</v>
       </c>
@@ -32379,8 +32530,11 @@
       <c r="E1302" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1302" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1303" t="s">
         <v>411</v>
       </c>
@@ -32397,8 +32551,11 @@
       <c r="E1303" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1303" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1304" t="s">
         <v>411</v>
       </c>
@@ -32415,8 +32572,11 @@
       <c r="E1304" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1304" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1305" t="s">
         <v>411</v>
       </c>
@@ -32433,8 +32593,11 @@
       <c r="E1305" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1305" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1306" t="s">
         <v>411</v>
       </c>
@@ -32451,8 +32614,11 @@
       <c r="E1306" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1306" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1307" t="s">
         <v>414</v>
       </c>
@@ -32469,8 +32635,11 @@
       <c r="E1307" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1307" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1308" t="s">
         <v>414</v>
       </c>
@@ -32487,8 +32656,11 @@
       <c r="E1308" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1308" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1309" t="s">
         <v>414</v>
       </c>
@@ -32505,8 +32677,11 @@
       <c r="E1309" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1309" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1310" t="s">
         <v>414</v>
       </c>
@@ -32523,8 +32698,11 @@
       <c r="E1310" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1311" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1310" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1311" t="s">
         <v>414</v>
       </c>
@@ -32541,8 +32719,11 @@
       <c r="E1311" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1311" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1312" t="s">
         <v>414</v>
       </c>
@@ -32559,8 +32740,11 @@
       <c r="E1312" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1312" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1313" t="s">
         <v>414</v>
       </c>
@@ -32577,8 +32761,11 @@
       <c r="E1313" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1313" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1314" t="s">
         <v>414</v>
       </c>
@@ -32595,8 +32782,11 @@
       <c r="E1314" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1314" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1315" t="s">
         <v>414</v>
       </c>
@@ -32613,8 +32803,11 @@
       <c r="E1315" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1315" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1316" t="s">
         <v>414</v>
       </c>
@@ -32631,8 +32824,11 @@
       <c r="E1316" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1316" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1317" t="s">
         <v>414</v>
       </c>
@@ -32649,8 +32845,11 @@
       <c r="E1317" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1317" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1318" t="s">
         <v>414</v>
       </c>
@@ -32667,8 +32866,11 @@
       <c r="E1318" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1318" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1319" t="s">
         <v>385</v>
       </c>
@@ -32685,8 +32887,11 @@
       <c r="E1319" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1320" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1319" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1320" t="s">
         <v>385</v>
       </c>
@@ -32703,8 +32908,11 @@
       <c r="E1320" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1321" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1320" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1321" t="s">
         <v>385</v>
       </c>
@@ -32721,8 +32929,11 @@
       <c r="E1321" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1322" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1321" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1322" t="s">
         <v>385</v>
       </c>
@@ -32739,8 +32950,11 @@
       <c r="E1322" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1323" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1322" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1323" t="s">
         <v>385</v>
       </c>
@@ -32757,8 +32971,11 @@
       <c r="E1323" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1324" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1323" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1324" t="s">
         <v>385</v>
       </c>
@@ -32775,8 +32992,11 @@
       <c r="E1324" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1325" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1324" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1325" t="s">
         <v>385</v>
       </c>
@@ -32793,8 +33013,11 @@
       <c r="E1325" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1325" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1326" t="s">
         <v>385</v>
       </c>
@@ -32811,8 +33034,11 @@
       <c r="E1326" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1326" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1327" t="s">
         <v>385</v>
       </c>
@@ -32829,8 +33055,11 @@
       <c r="E1327" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1327" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1328" t="s">
         <v>385</v>
       </c>
@@ -32847,8 +33076,11 @@
       <c r="E1328" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1329" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1328" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1329" t="s">
         <v>385</v>
       </c>
@@ -32865,8 +33097,11 @@
       <c r="E1329" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1329" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1330" t="s">
         <v>385</v>
       </c>
@@ -32883,8 +33118,11 @@
       <c r="E1330" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1330" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1331" t="s">
         <v>385</v>
       </c>
@@ -32901,8 +33139,11 @@
       <c r="E1331" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1331" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1332" t="s">
         <v>385</v>
       </c>
@@ -32919,8 +33160,11 @@
       <c r="E1332" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1332" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1333" t="s">
         <v>385</v>
       </c>
@@ -32937,8 +33181,11 @@
       <c r="E1333" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1333" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1334" t="s">
         <v>385</v>
       </c>
@@ -32955,8 +33202,11 @@
       <c r="E1334" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1334" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1335" t="s">
         <v>385</v>
       </c>
@@ -32973,8 +33223,11 @@
       <c r="E1335" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1335" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1336" t="s">
         <v>385</v>
       </c>
@@ -32991,8 +33244,11 @@
       <c r="E1336" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1336" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1337" t="s">
         <v>385</v>
       </c>
@@ -33009,8 +33265,11 @@
       <c r="E1337" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1337" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1338" t="s">
         <v>388</v>
       </c>
@@ -33027,8 +33286,11 @@
       <c r="E1338" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1338" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1339" t="s">
         <v>388</v>
       </c>
@@ -33045,8 +33307,11 @@
       <c r="E1339" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1339" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1340" t="s">
         <v>388</v>
       </c>
@@ -33063,8 +33328,11 @@
       <c r="E1340" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1341" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1340" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1341" t="s">
         <v>388</v>
       </c>
@@ -33081,8 +33349,11 @@
       <c r="E1341" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1342" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1341" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1342" t="s">
         <v>388</v>
       </c>
@@ -33099,8 +33370,11 @@
       <c r="E1342" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1343" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1342" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1343" t="s">
         <v>388</v>
       </c>
@@ -33117,8 +33391,11 @@
       <c r="E1343" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1343" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1344" t="s">
         <v>388</v>
       </c>
@@ -33135,8 +33412,11 @@
       <c r="E1344" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1344" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1345" t="s">
         <v>388</v>
       </c>
@@ -33153,8 +33433,11 @@
       <c r="E1345" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1346" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1345" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1346" t="s">
         <v>388</v>
       </c>
@@ -33171,8 +33454,11 @@
       <c r="E1346" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1347" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1346" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1347" t="s">
         <v>388</v>
       </c>
@@ -33189,8 +33475,11 @@
       <c r="E1347" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1348" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1347" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1348" t="s">
         <v>388</v>
       </c>
@@ -33207,8 +33496,11 @@
       <c r="E1348" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1349" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1348" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1349" t="s">
         <v>388</v>
       </c>
@@ -33225,8 +33517,11 @@
       <c r="E1349" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1350" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1349" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1350" t="s">
         <v>388</v>
       </c>
@@ -33243,8 +33538,11 @@
       <c r="E1350" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1351" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1350" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1351" t="s">
         <v>388</v>
       </c>
@@ -33261,8 +33559,11 @@
       <c r="E1351" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1352" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1351" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1352" t="s">
         <v>388</v>
       </c>
@@ -33279,8 +33580,11 @@
       <c r="E1352" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1353" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1352" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1353" t="s">
         <v>388</v>
       </c>
@@ -33297,8 +33601,11 @@
       <c r="E1353" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1354" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1353" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1354" t="s">
         <v>388</v>
       </c>
@@ -33315,8 +33622,11 @@
       <c r="E1354" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1355" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1354" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1355" t="s">
         <v>391</v>
       </c>
@@ -33333,8 +33643,11 @@
       <c r="E1355" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1356" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1355" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1356" t="s">
         <v>391</v>
       </c>
@@ -33351,8 +33664,11 @@
       <c r="E1356" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1357" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1356" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1357" t="s">
         <v>391</v>
       </c>
@@ -33369,8 +33685,11 @@
       <c r="E1357" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1358" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1357" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1358" t="s">
         <v>391</v>
       </c>
@@ -33387,8 +33706,11 @@
       <c r="E1358" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1359" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1358" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1359" t="s">
         <v>391</v>
       </c>
@@ -33405,8 +33727,11 @@
       <c r="E1359" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1360" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1359" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1360" t="s">
         <v>391</v>
       </c>
@@ -33423,8 +33748,11 @@
       <c r="E1360" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1361" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1360" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1361" t="s">
         <v>391</v>
       </c>
@@ -33441,8 +33769,11 @@
       <c r="E1361" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1362" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1361" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1362" t="s">
         <v>391</v>
       </c>
@@ -33459,8 +33790,11 @@
       <c r="E1362" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1363" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1362" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1363" t="s">
         <v>391</v>
       </c>
@@ -33477,8 +33811,11 @@
       <c r="E1363" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1364" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1363" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1364" t="s">
         <v>391</v>
       </c>
@@ -33495,8 +33832,11 @@
       <c r="E1364" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1364" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1365" t="s">
         <v>391</v>
       </c>
@@ -33513,8 +33853,11 @@
       <c r="E1365" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1365" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1366" t="s">
         <v>391</v>
       </c>
@@ -33531,8 +33874,11 @@
       <c r="E1366" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1367" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1366" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1367" t="s">
         <v>391</v>
       </c>
@@ -33549,8 +33895,11 @@
       <c r="E1367" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1368" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1367" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1368" t="s">
         <v>391</v>
       </c>
@@ -33567,8 +33916,11 @@
       <c r="E1368" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1368" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1369" t="s">
         <v>391</v>
       </c>
@@ -33585,8 +33937,11 @@
       <c r="E1369" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1370" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1369" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1370" t="s">
         <v>391</v>
       </c>
@@ -33603,8 +33958,11 @@
       <c r="E1370" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1370" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1371" t="s">
         <v>394</v>
       </c>
@@ -33621,8 +33979,11 @@
       <c r="E1371" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1372" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1371" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1372" t="s">
         <v>394</v>
       </c>
@@ -33639,8 +34000,11 @@
       <c r="E1372" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1373" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1372" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1373" t="s">
         <v>394</v>
       </c>
@@ -33657,8 +34021,11 @@
       <c r="E1373" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1374" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1373" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1374" t="s">
         <v>394</v>
       </c>
@@ -33675,8 +34042,11 @@
       <c r="E1374" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1375" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1374" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1375" t="s">
         <v>394</v>
       </c>
@@ -33693,8 +34063,11 @@
       <c r="E1375" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1376" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1375" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1376" t="s">
         <v>394</v>
       </c>
@@ -33711,8 +34084,11 @@
       <c r="E1376" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1376" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1377" t="s">
         <v>394</v>
       </c>
@@ -33729,8 +34105,11 @@
       <c r="E1377" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1377" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1378" t="s">
         <v>394</v>
       </c>
@@ -33747,8 +34126,11 @@
       <c r="E1378" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1378" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1379" t="s">
         <v>394</v>
       </c>
@@ -33765,8 +34147,11 @@
       <c r="E1379" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1380" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1379" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1380" t="s">
         <v>394</v>
       </c>
@@ -33783,8 +34168,11 @@
       <c r="E1380" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1381" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1380" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1381" t="s">
         <v>394</v>
       </c>
@@ -33801,8 +34189,11 @@
       <c r="E1381" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1382" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1381" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1382" t="s">
         <v>394</v>
       </c>
@@ -33819,8 +34210,11 @@
       <c r="E1382" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1383" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1382" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1383" t="s">
         <v>394</v>
       </c>
@@ -33837,8 +34231,11 @@
       <c r="E1383" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1383" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1384" t="s">
         <v>394</v>
       </c>
@@ -33855,8 +34252,11 @@
       <c r="E1384" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1385" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1384" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1385" t="s">
         <v>394</v>
       </c>
@@ -33873,8 +34273,11 @@
       <c r="E1385" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1385" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1386" t="s">
         <v>394</v>
       </c>
@@ -33891,8 +34294,11 @@
       <c r="E1386" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1386" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1387" t="s">
         <v>394</v>
       </c>
@@ -33909,8 +34315,11 @@
       <c r="E1387" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1387" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1388" t="s">
         <v>394</v>
       </c>
@@ -33927,8 +34336,11 @@
       <c r="E1388" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1388" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1389" t="s">
         <v>394</v>
       </c>
@@ -33945,8 +34357,11 @@
       <c r="E1389" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1389" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1390" t="s">
         <v>394</v>
       </c>
@@ -33963,8 +34378,11 @@
       <c r="E1390" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1390" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1391" t="s">
         <v>394</v>
       </c>
@@ -33981,8 +34399,11 @@
       <c r="E1391" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1391" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1392" t="s">
         <v>394</v>
       </c>
@@ -33999,8 +34420,11 @@
       <c r="E1392" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1392" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1393" t="s">
         <v>394</v>
       </c>
@@ -34017,8 +34441,11 @@
       <c r="E1393" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1393" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1394" t="s">
         <v>394</v>
       </c>
@@ -34035,8 +34462,11 @@
       <c r="E1394" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1394" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1395" t="s">
         <v>394</v>
       </c>
@@ -34053,8 +34483,11 @@
       <c r="E1395" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1395" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1396" t="s">
         <v>394</v>
       </c>
@@ -34071,8 +34504,11 @@
       <c r="E1396" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1396" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1397" t="s">
         <v>394</v>
       </c>
@@ -34089,8 +34525,11 @@
       <c r="E1397" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1397" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1398" t="s">
         <v>394</v>
       </c>
@@ -34107,8 +34546,11 @@
       <c r="E1398" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1398" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1399" t="s">
         <v>394</v>
       </c>
@@ -34125,8 +34567,11 @@
       <c r="E1399" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1399" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1400" t="s">
         <v>394</v>
       </c>
@@ -34143,8 +34588,11 @@
       <c r="E1400" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1401" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1400" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1401" t="s">
         <v>394</v>
       </c>
@@ -34161,8 +34609,11 @@
       <c r="E1401" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1402" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1401" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1402" t="s">
         <v>394</v>
       </c>
@@ -34179,8 +34630,11 @@
       <c r="E1402" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1403" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1402" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1403" t="s">
         <v>394</v>
       </c>
@@ -34197,8 +34651,11 @@
       <c r="E1403" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1404" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1403" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1404" t="s">
         <v>394</v>
       </c>
@@ -34215,8 +34672,11 @@
       <c r="E1404" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1405" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1404" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1405" t="s">
         <v>394</v>
       </c>
@@ -34233,8 +34693,11 @@
       <c r="E1405" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1406" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1405" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1406" t="s">
         <v>394</v>
       </c>
@@ -34251,8 +34714,11 @@
       <c r="E1406" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1407" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1406" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1407" t="s">
         <v>397</v>
       </c>
@@ -34269,8 +34735,11 @@
       <c r="E1407" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1408" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1407" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1408" t="s">
         <v>397</v>
       </c>
@@ -34287,8 +34756,11 @@
       <c r="E1408" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1409" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1408" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1409" t="s">
         <v>397</v>
       </c>
@@ -34305,8 +34777,11 @@
       <c r="E1409" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1410" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1409" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1410" t="s">
         <v>397</v>
       </c>
@@ -34323,8 +34798,11 @@
       <c r="E1410" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1411" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1410" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1411" t="s">
         <v>397</v>
       </c>
@@ -34341,8 +34819,11 @@
       <c r="E1411" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1412" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1411" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1412" t="s">
         <v>397</v>
       </c>
@@ -34359,8 +34840,11 @@
       <c r="E1412" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1413" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1412" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1413" t="s">
         <v>397</v>
       </c>
@@ -34377,8 +34861,11 @@
       <c r="E1413" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1414" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1413" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1414" t="s">
         <v>397</v>
       </c>
@@ -34395,8 +34882,11 @@
       <c r="E1414" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1415" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1414" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1415" t="s">
         <v>399</v>
       </c>
@@ -34413,8 +34903,11 @@
       <c r="E1415" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="1416" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1415" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1416" t="s">
         <v>399</v>
       </c>
@@ -34431,8 +34924,11 @@
       <c r="E1416" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1417" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1416" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1417" t="s">
         <v>399</v>
       </c>
@@ -34449,8 +34945,11 @@
       <c r="E1417" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1418" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1417" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1418" t="s">
         <v>399</v>
       </c>
@@ -34467,8 +34966,11 @@
       <c r="E1418" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1419" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1418" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1419" t="s">
         <v>399</v>
       </c>
@@ -34485,8 +34987,11 @@
       <c r="E1419" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1420" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1419" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1420" t="s">
         <v>399</v>
       </c>
@@ -34503,8 +35008,11 @@
       <c r="E1420" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1421" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1420" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1421" t="s">
         <v>399</v>
       </c>
@@ -34521,8 +35029,11 @@
       <c r="E1421" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1422" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1421" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1422" t="s">
         <v>399</v>
       </c>
@@ -34539,8 +35050,11 @@
       <c r="E1422" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1423" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1422" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1423" t="s">
         <v>399</v>
       </c>
@@ -34557,8 +35071,11 @@
       <c r="E1423" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1424" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1423" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1424" t="s">
         <v>399</v>
       </c>
@@ -34575,8 +35092,11 @@
       <c r="E1424" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1425" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1424" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1425" t="s">
         <v>399</v>
       </c>
@@ -34593,8 +35113,11 @@
       <c r="E1425" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1426" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1425" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1426" t="s">
         <v>399</v>
       </c>
@@ -34611,8 +35134,11 @@
       <c r="E1426" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1427" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1426" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1427" t="s">
         <v>399</v>
       </c>
@@ -34629,8 +35155,11 @@
       <c r="E1427" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1428" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1427" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1428" t="s">
         <v>399</v>
       </c>
@@ -34647,8 +35176,11 @@
       <c r="E1428" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1429" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1428" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1429" t="s">
         <v>399</v>
       </c>
@@ -34665,8 +35197,11 @@
       <c r="E1429" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1430" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1429" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1430" t="s">
         <v>399</v>
       </c>
@@ -34683,8 +35218,11 @@
       <c r="E1430" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1431" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1430" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1431" t="s">
         <v>399</v>
       </c>
@@ -34701,8 +35239,11 @@
       <c r="E1431" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1432" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1431" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1432" t="s">
         <v>399</v>
       </c>
@@ -34719,8 +35260,11 @@
       <c r="E1432" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1433" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1432" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1433" t="s">
         <v>399</v>
       </c>
@@ -34737,8 +35281,11 @@
       <c r="E1433" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1434" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1433" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1434" t="s">
         <v>399</v>
       </c>
@@ -34755,8 +35302,11 @@
       <c r="E1434" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1435" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1434" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1435" t="s">
         <v>399</v>
       </c>
@@ -34773,8 +35323,11 @@
       <c r="E1435" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1436" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1435" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1436" t="s">
         <v>399</v>
       </c>
@@ -34791,8 +35344,11 @@
       <c r="E1436" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1437" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1436" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1437" t="s">
         <v>399</v>
       </c>
@@ -34809,8 +35365,11 @@
       <c r="E1437" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1438" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1437" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1438" t="s">
         <v>399</v>
       </c>
@@ -34827,8 +35386,11 @@
       <c r="E1438" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1439" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1438" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1439" t="s">
         <v>399</v>
       </c>
@@ -34845,8 +35407,11 @@
       <c r="E1439" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1440" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1439" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1440" t="s">
         <v>399</v>
       </c>
@@ -34863,8 +35428,11 @@
       <c r="E1440" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1441" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1440" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1441" t="s">
         <v>399</v>
       </c>
@@ -34881,8 +35449,11 @@
       <c r="E1441" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="1442" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1441" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1442" t="s">
         <v>399</v>
       </c>
@@ -34899,8 +35470,11 @@
       <c r="E1442" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1443" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1442" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1443" t="s">
         <v>399</v>
       </c>
@@ -34917,8 +35491,11 @@
       <c r="E1443" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="1444" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1443" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1444" t="s">
         <v>399</v>
       </c>
@@ -34935,8 +35512,11 @@
       <c r="E1444" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="1445" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1444" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1445" t="s">
         <v>932</v>
       </c>
@@ -34954,7 +35534,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="1446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1446" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1446" t="s">
         <v>932</v>
       </c>
@@ -34972,7 +35552,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="1447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1447" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1447" t="s">
         <v>932</v>
       </c>
@@ -34990,7 +35570,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="1448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1448" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1448" t="s">
         <v>932</v>
       </c>
@@ -35008,7 +35588,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="1449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1449" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1449" t="s">
         <v>932</v>
       </c>
@@ -35026,7 +35606,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="1450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1450" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1450" t="s">
         <v>932</v>
       </c>
@@ -35044,7 +35624,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="1451" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1451" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1451" t="s">
         <v>932</v>
       </c>
@@ -35062,7 +35642,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="1452" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1452" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1452" t="s">
         <v>932</v>
       </c>
@@ -35080,7 +35660,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="1453" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1453" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1453" t="s">
         <v>932</v>
       </c>
@@ -35098,7 +35678,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="1454" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1454" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1454" t="s">
         <v>932</v>
       </c>
@@ -35116,7 +35696,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="1455" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1455" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1455" t="s">
         <v>932</v>
       </c>
@@ -35134,7 +35714,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="1456" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1456" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1456" t="s">
         <v>932</v>
       </c>

</xml_diff>

<commit_message>
Creacion de script de tablas silesweb
</commit_message>
<xml_diff>
--- a/SILESWEB/DOCUMENTACION/Estructura de las tablas.xlsx
+++ b/SILESWEB/DOCUMENTACION/Estructura de las tablas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SILESWEB\SILESWEB\DOCUMENTACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredy Sarmiento\Documents\SilesWeb\SILESWEB\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D490F2B-60F0-419A-9970-6319E76D1D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="2" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Hoja1" sheetId="4" r:id="rId3"/>
     <sheet name="Convenciones" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12006" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12006" uniqueCount="1044">
   <si>
     <t>nIdPEROP</t>
   </si>
@@ -3182,11 +3181,14 @@
   <si>
     <t>TL_FIN_TNSA_NiifSaldosTerceros</t>
   </si>
+  <si>
+    <t>TL_FIN_TSAC_SaldosInicialesTerceros</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3305,14 +3307,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:F2018" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:F2018" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TABLA"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Nombre_tabla" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE_CAMPO"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TIPO DE DATOS"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TIPO DE DATOS SQL"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nueva Tabla"/>
+    <tableColumn id="1" name="TABLA"/>
+    <tableColumn id="4" name="Nombre_tabla" dataDxfId="0"/>
+    <tableColumn id="2" name="NOMBRE_CAMPO"/>
+    <tableColumn id="3" name="TIPO DE DATOS"/>
+    <tableColumn id="5" name="TIPO DE DATOS SQL"/>
+    <tableColumn id="6" name="Nueva Tabla"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3580,11 +3582,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B905" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F923" sqref="F923"/>
+    <sheetView tabSelected="1" topLeftCell="C1010" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1018" sqref="E1018"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21951,7 +21953,7 @@
         <v>808</v>
       </c>
       <c r="F927" t="s">
-        <v>882</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="928" spans="1:6" x14ac:dyDescent="0.25">
@@ -21971,7 +21973,7 @@
         <v>803</v>
       </c>
       <c r="F928" t="s">
-        <v>882</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="929" spans="1:6" x14ac:dyDescent="0.25">
@@ -21991,7 +21993,7 @@
         <v>803</v>
       </c>
       <c r="F929" t="s">
-        <v>882</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="930" spans="1:6" x14ac:dyDescent="0.25">
@@ -22011,7 +22013,7 @@
         <v>803</v>
       </c>
       <c r="F930" t="s">
-        <v>882</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="931" spans="1:6" x14ac:dyDescent="0.25">
@@ -22031,7 +22033,7 @@
         <v>806</v>
       </c>
       <c r="F931" t="s">
-        <v>882</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="932" spans="1:6" x14ac:dyDescent="0.25">
@@ -22051,7 +22053,7 @@
         <v>806</v>
       </c>
       <c r="F932" t="s">
-        <v>882</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="933" spans="1:6" x14ac:dyDescent="0.25">
@@ -43725,7 +43727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43771,7 +43773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -44338,7 +44340,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
avance 2 de sql
</commit_message>
<xml_diff>
--- a/SILESWEB/DOCUMENTACION/Estructura de las tablas.xlsx
+++ b/SILESWEB/DOCUMENTACION/Estructura de las tablas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fredy Sarmiento\Documents\SilesWeb\SILESWEB\DOCUMENTACION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SILESWEB\SILESWEB\DOCUMENTACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD23A0-4AA9-4ACE-8F87-CC687800D3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="2" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Hoja1" sheetId="4" r:id="rId3"/>
     <sheet name="Convenciones" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12006" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12007" uniqueCount="1044">
   <si>
     <t>nIdPEROP</t>
   </si>
@@ -3188,7 +3189,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3307,14 +3308,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:F2018" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla2" displayName="Tabla2" ref="A1:F2018" totalsRowShown="0">
   <tableColumns count="6">
-    <tableColumn id="1" name="TABLA"/>
-    <tableColumn id="4" name="Nombre_tabla" dataDxfId="0"/>
-    <tableColumn id="2" name="NOMBRE_CAMPO"/>
-    <tableColumn id="3" name="TIPO DE DATOS"/>
-    <tableColumn id="5" name="TIPO DE DATOS SQL"/>
-    <tableColumn id="6" name="Nueva Tabla"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TABLA"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Nombre_tabla" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NOMBRE_CAMPO"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TIPO DE DATOS"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="TIPO DE DATOS SQL"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nueva Tabla"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3582,11 +3583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1010" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1018" sqref="E1018"/>
+    <sheetView tabSelected="1" topLeftCell="A1401" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1417" sqref="C1417:C1436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31456,6 +31457,9 @@
       <c r="E1405" t="s">
         <v>806</v>
       </c>
+      <c r="F1405" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="1406" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1406" t="s">
@@ -43727,7 +43731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43773,7 +43777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -44340,7 +44344,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>